<commit_message>
tratamento, quando valor de planilha não é do tipo condizente com a conversão
</commit_message>
<xml_diff>
--- a/import.xlsx
+++ b/import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\labs\dotnet\LerPlanilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0947EFF0-C30B-4316-B2DA-1ACD2B06B02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BB0877-D487-4914-8111-8D5D7BBDE4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{117D67C4-8162-4B56-9069-59FAB19D63C4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Computador Desktop</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Monitor 24"</t>
+  </si>
+  <si>
+    <t>LEANDRO</t>
   </si>
 </sst>
 </file>
@@ -413,14 +416,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:I1048576"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -463,8 +466,8 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4">
-        <v>150</v>
+      <c r="C4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>